<commit_message>
rfq table broken links fix
</commit_message>
<xml_diff>
--- a/export_pr.xlsx
+++ b/export_pr.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
   <si>
     <t>Appendix 60</t>
   </si>
@@ -38,13 +38,13 @@
     <t>FAD</t>
   </si>
   <si>
-    <t>PR No.:  2020-02-00123</t>
+    <t>PR No.:  2020-03-0133</t>
   </si>
   <si>
     <t xml:space="preserve">Date: </t>
   </si>
   <si>
-    <t>February 28, 2020</t>
+    <t>March 02, 2020</t>
   </si>
   <si>
     <t xml:space="preserve">Responsibility Center Code : </t>
@@ -68,14 +68,21 @@
     <t>Total Cost</t>
   </si>
   <si>
-    <t>S454</t>
-  </si>
-  <si>
-    <t>lot</t>
-  </si>
-  <si>
-    <t>Isuzu Crosswind CN8994
-alternator and aircon belt</t>
+    <t>S273</t>
+  </si>
+  <si>
+    <t>piece</t>
+  </si>
+  <si>
+    <t>Archfile Folder, Legal
+* 2" /3" spine 2 rings</t>
+  </si>
+  <si>
+    <t>S298</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signpen, 0.7, Blue
+</t>
   </si>
   <si>
     <t>Total</t>
@@ -84,7 +91,7 @@
     <t>Purpose:</t>
   </si>
   <si>
-    <t>Replacement of defective alternator and aircon belt of DILG Service Vehicle</t>
+    <t>Realignment of Regional Records Management (QP-R4A-FAD-RICTU-08) to the newly developed Document Management System (DMS)</t>
   </si>
   <si>
     <t>Requested by:</t>
@@ -118,9 +125,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00;[Red]#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -338,25 +344,25 @@
       </bottom>
     </border>
     <border>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
-    </border>
-    <border>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="2" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection hidden="false"/>
@@ -469,10 +475,6 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
-    <xf xfId="0" fontId="3" numFmtId="165" fillId="2" borderId="5" applyFont="1" applyNumberFormat="1" applyFill="0" applyBorder="1" applyAlignment="0" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="7" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection hidden="false"/>
@@ -481,6 +483,94 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="12" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="13" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="14" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="15" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false" indent="3"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="16" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false" indent="3"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="16" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="15" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="15" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="16" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="14" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
     <xf xfId="0" fontId="5" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection hidden="false"/>
@@ -497,14 +587,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="12" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="13" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
     <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection hidden="false"/>
@@ -521,84 +603,12 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false" indent="3"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="14" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false" indent="3"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="14" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="15" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="15" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="14" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="16" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="2" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="3" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="16" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="4" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="15" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
-      <protection hidden="false"/>
-    </xf>
-    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
+      <protection hidden="false"/>
+    </xf>
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="2" borderId="5" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
       <protection hidden="false"/>
     </xf>
   </cellXfs>
@@ -904,7 +914,7 @@
   <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" view="pageBreakPreview" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="D43" sqref="D43"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="true" defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -919,10 +929,10 @@
   <sheetData>
     <row r="1" spans="1:6" customHeight="1" ht="15.75">
       <c r="A1" s="1"/>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="31"/>
+      <c r="F1" s="52"/>
     </row>
     <row r="2" spans="1:6" customHeight="1" ht="18.75">
       <c r="A2" s="1"/>
@@ -930,30 +940,30 @@
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" customHeight="1" ht="18.75">
-      <c r="A3" s="39"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
+      <c r="A3" s="58"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
     </row>
     <row r="4" spans="1:6" customHeight="1" ht="18.75">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="58"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
     </row>
     <row r="5" spans="1:6" customHeight="1" ht="15.75">
-      <c r="A5" s="40"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
     </row>
     <row r="6" spans="1:6" customHeight="1" ht="21" s="7" customFormat="1">
       <c r="A6" s="8" t="s">
@@ -963,11 +973,11 @@
         <v>3</v>
       </c>
       <c r="C6" s="9"/>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
     </row>
     <row r="7" spans="1:6" customHeight="1" ht="18" s="7" customFormat="1">
       <c r="A7" s="14" t="s">
@@ -980,16 +990,16 @@
         <v>7</v>
       </c>
       <c r="D7" s="13"/>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="F7" s="61" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:6" customHeight="1" ht="30.75" s="7" customFormat="1">
-      <c r="A8" s="37"/>
-      <c r="B8" s="38"/>
+      <c r="A8" s="56"/>
+      <c r="B8" s="57"/>
       <c r="C8" s="15" t="s">
         <v>10</v>
       </c>
@@ -998,32 +1008,32 @@
       <c r="F8" s="10"/>
     </row>
     <row r="9" spans="1:6" customHeight="1" ht="16.5" s="7" customFormat="1">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="35" t="s">
+      <c r="F9" s="30" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:6" customHeight="1" ht="15.75" s="7" customFormat="1">
-      <c r="A10" s="34"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="A10" s="55"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
     </row>
     <row r="11" spans="1:6" customHeight="1" ht="30" s="2" customFormat="1">
       <c r="A11" s="17" t="s">
@@ -1032,31 +1042,43 @@
       <c r="B11" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="28" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="18">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E11" s="26">
-        <v>3000</v>
+        <v>300</v>
       </c>
       <c r="F11" s="26">
-        <v>3000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="12" spans="1:6" customHeight="1" ht="30" s="2" customFormat="1">
-      <c r="A12" s="19"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
+      <c r="A12" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="20">
+        <v>5</v>
+      </c>
+      <c r="E12" s="27">
+        <v>100</v>
+      </c>
+      <c r="F12" s="27">
+        <v>500</v>
+      </c>
     </row>
     <row r="13" spans="1:6" customHeight="1" ht="30" s="2" customFormat="1">
       <c r="A13" s="19"/>
       <c r="B13" s="20"/>
-      <c r="C13" s="30"/>
+      <c r="C13" s="29"/>
       <c r="D13" s="20"/>
       <c r="E13" s="27"/>
       <c r="F13" s="27"/>
@@ -1064,7 +1086,7 @@
     <row r="14" spans="1:6" customHeight="1" ht="30" s="2" customFormat="1">
       <c r="A14" s="19"/>
       <c r="B14" s="20"/>
-      <c r="C14" s="30"/>
+      <c r="C14" s="29"/>
       <c r="D14" s="20"/>
       <c r="E14" s="27"/>
       <c r="F14" s="27"/>
@@ -1072,7 +1094,7 @@
     <row r="15" spans="1:6" customHeight="1" ht="30" s="2" customFormat="1">
       <c r="A15" s="19"/>
       <c r="B15" s="20"/>
-      <c r="C15" s="30"/>
+      <c r="C15" s="29"/>
       <c r="D15" s="20"/>
       <c r="E15" s="27"/>
       <c r="F15" s="27"/>
@@ -1080,7 +1102,7 @@
     <row r="16" spans="1:6" customHeight="1" ht="30" s="2" customFormat="1">
       <c r="A16" s="19"/>
       <c r="B16" s="20"/>
-      <c r="C16" s="30"/>
+      <c r="C16" s="29"/>
       <c r="D16" s="20"/>
       <c r="E16" s="27"/>
       <c r="F16" s="27"/>
@@ -1088,7 +1110,7 @@
     <row r="17" spans="1:6" customHeight="1" ht="30" s="2" customFormat="1">
       <c r="A17" s="19"/>
       <c r="B17" s="20"/>
-      <c r="C17" s="30"/>
+      <c r="C17" s="29"/>
       <c r="D17" s="20"/>
       <c r="E17" s="27"/>
       <c r="F17" s="27"/>
@@ -1096,7 +1118,7 @@
     <row r="18" spans="1:6" customHeight="1" ht="30" s="2" customFormat="1">
       <c r="A18" s="19"/>
       <c r="B18" s="20"/>
-      <c r="C18" s="30"/>
+      <c r="C18" s="29"/>
       <c r="D18" s="20"/>
       <c r="E18" s="27"/>
       <c r="F18" s="27"/>
@@ -1104,7 +1126,7 @@
     <row r="19" spans="1:6" customHeight="1" ht="30" s="2" customFormat="1">
       <c r="A19" s="19"/>
       <c r="B19" s="20"/>
-      <c r="C19" s="30"/>
+      <c r="C19" s="29"/>
       <c r="D19" s="20"/>
       <c r="E19" s="27"/>
       <c r="F19" s="27"/>
@@ -1112,7 +1134,7 @@
     <row r="20" spans="1:6" customHeight="1" ht="30" s="2" customFormat="1">
       <c r="A20" s="19"/>
       <c r="B20" s="20"/>
-      <c r="C20" s="30"/>
+      <c r="C20" s="29"/>
       <c r="D20" s="20"/>
       <c r="E20" s="27"/>
       <c r="F20" s="27"/>
@@ -1120,7 +1142,7 @@
     <row r="21" spans="1:6" customHeight="1" ht="30" s="2" customFormat="1">
       <c r="A21" s="19"/>
       <c r="B21" s="20"/>
-      <c r="C21" s="30"/>
+      <c r="C21" s="29"/>
       <c r="D21" s="20"/>
       <c r="E21" s="27"/>
       <c r="F21" s="27"/>
@@ -1128,7 +1150,7 @@
     <row r="22" spans="1:6" customHeight="1" ht="30" s="2" customFormat="1">
       <c r="A22" s="19"/>
       <c r="B22" s="20"/>
-      <c r="C22" s="30"/>
+      <c r="C22" s="29"/>
       <c r="D22" s="20"/>
       <c r="E22" s="27"/>
       <c r="F22" s="27"/>
@@ -1136,7 +1158,7 @@
     <row r="23" spans="1:6" customHeight="1" ht="30" s="2" customFormat="1">
       <c r="A23" s="19"/>
       <c r="B23" s="20"/>
-      <c r="C23" s="30"/>
+      <c r="C23" s="29"/>
       <c r="D23" s="20"/>
       <c r="E23" s="27"/>
       <c r="F23" s="27"/>
@@ -1144,7 +1166,7 @@
     <row r="24" spans="1:6" customHeight="1" ht="30" s="2" customFormat="1">
       <c r="A24" s="19"/>
       <c r="B24" s="20"/>
-      <c r="C24" s="30"/>
+      <c r="C24" s="29"/>
       <c r="D24" s="20"/>
       <c r="E24" s="27"/>
       <c r="F24" s="27"/>
@@ -1152,7 +1174,7 @@
     <row r="25" spans="1:6" customHeight="1" ht="30" s="2" customFormat="1">
       <c r="A25" s="19"/>
       <c r="B25" s="20"/>
-      <c r="C25" s="30"/>
+      <c r="C25" s="29"/>
       <c r="D25" s="20"/>
       <c r="E25" s="27"/>
       <c r="F25" s="27"/>
@@ -1160,7 +1182,7 @@
     <row r="26" spans="1:6" customHeight="1" ht="30" s="2" customFormat="1">
       <c r="A26" s="19"/>
       <c r="B26" s="20"/>
-      <c r="C26" s="30"/>
+      <c r="C26" s="29"/>
       <c r="D26" s="20"/>
       <c r="E26" s="27"/>
       <c r="F26" s="27"/>
@@ -1168,7 +1190,7 @@
     <row r="27" spans="1:6" customHeight="1" ht="30" s="2" customFormat="1">
       <c r="A27" s="19"/>
       <c r="B27" s="20"/>
-      <c r="C27" s="30"/>
+      <c r="C27" s="29"/>
       <c r="D27" s="20"/>
       <c r="E27" s="27"/>
       <c r="F27" s="27"/>
@@ -1176,7 +1198,7 @@
     <row r="28" spans="1:6" customHeight="1" ht="30" s="2" customFormat="1">
       <c r="A28" s="19"/>
       <c r="B28" s="20"/>
-      <c r="C28" s="30"/>
+      <c r="C28" s="29"/>
       <c r="D28" s="20"/>
       <c r="E28" s="27"/>
       <c r="F28" s="27"/>
@@ -1184,7 +1206,7 @@
     <row r="29" spans="1:6" customHeight="1" ht="30" s="2" customFormat="1">
       <c r="A29" s="19"/>
       <c r="B29" s="20"/>
-      <c r="C29" s="30"/>
+      <c r="C29" s="29"/>
       <c r="D29" s="20"/>
       <c r="E29" s="27"/>
       <c r="F29" s="27"/>
@@ -1192,7 +1214,7 @@
     <row r="30" spans="1:6" customHeight="1" ht="30" s="2" customFormat="1">
       <c r="A30" s="19"/>
       <c r="B30" s="20"/>
-      <c r="C30" s="30"/>
+      <c r="C30" s="29"/>
       <c r="D30" s="20"/>
       <c r="E30" s="27"/>
       <c r="F30" s="27"/>
@@ -1200,7 +1222,7 @@
     <row r="31" spans="1:6" customHeight="1" ht="30" s="2" customFormat="1">
       <c r="A31" s="19"/>
       <c r="B31" s="20"/>
-      <c r="C31" s="30"/>
+      <c r="C31" s="29"/>
       <c r="D31" s="20"/>
       <c r="E31" s="27"/>
       <c r="F31" s="27"/>
@@ -1208,7 +1230,7 @@
     <row r="32" spans="1:6" customHeight="1" ht="30" s="2" customFormat="1">
       <c r="A32" s="19"/>
       <c r="B32" s="20"/>
-      <c r="C32" s="30"/>
+      <c r="C32" s="29"/>
       <c r="D32" s="20"/>
       <c r="E32" s="27"/>
       <c r="F32" s="27"/>
@@ -1216,7 +1238,7 @@
     <row r="33" spans="1:6" customHeight="1" ht="30" s="2" customFormat="1">
       <c r="A33" s="19"/>
       <c r="B33" s="20"/>
-      <c r="C33" s="30"/>
+      <c r="C33" s="29"/>
       <c r="D33" s="20"/>
       <c r="E33" s="27"/>
       <c r="F33" s="27"/>
@@ -1224,7 +1246,7 @@
     <row r="34" spans="1:6" customHeight="1" ht="30" s="2" customFormat="1">
       <c r="A34" s="19"/>
       <c r="B34" s="20"/>
-      <c r="C34" s="30"/>
+      <c r="C34" s="29"/>
       <c r="D34" s="20"/>
       <c r="E34" s="27"/>
       <c r="F34" s="27"/>
@@ -1232,7 +1254,7 @@
     <row r="35" spans="1:6" customHeight="1" ht="30" s="2" customFormat="1">
       <c r="A35" s="19"/>
       <c r="B35" s="20"/>
-      <c r="C35" s="30"/>
+      <c r="C35" s="29"/>
       <c r="D35" s="20"/>
       <c r="E35" s="27"/>
       <c r="F35" s="27"/>
@@ -1243,114 +1265,103 @@
       <c r="C36" s="22"/>
       <c r="D36" s="22"/>
       <c r="E36" s="24" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F36" s="25">
         <f>SUM(F11:F35)</f>
-        <v>3000</v>
+        <v>6500</v>
       </c>
     </row>
     <row r="37" spans="1:6" customHeight="1" ht="15.75">
-      <c r="A37" s="53" t="s">
-        <v>21</v>
-      </c>
-      <c r="B37" s="47" t="s">
-        <v>22</v>
-      </c>
-      <c r="C37" s="47"/>
-      <c r="D37" s="47"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="48"/>
+      <c r="A37" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="42"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="43"/>
     </row>
     <row r="38" spans="1:6" customHeight="1" ht="15.75">
-      <c r="A38" s="54"/>
-      <c r="B38" s="49"/>
-      <c r="C38" s="49"/>
-      <c r="D38" s="49"/>
-      <c r="E38" s="49"/>
-      <c r="F38" s="50"/>
+      <c r="A38" s="48"/>
+      <c r="B38" s="44"/>
+      <c r="C38" s="44"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="45"/>
     </row>
     <row r="39" spans="1:6" customHeight="1" ht="15.75">
-      <c r="A39" s="54"/>
-      <c r="B39" s="49"/>
-      <c r="C39" s="49"/>
-      <c r="D39" s="49"/>
-      <c r="E39" s="49"/>
-      <c r="F39" s="50"/>
+      <c r="A39" s="48"/>
+      <c r="B39" s="44"/>
+      <c r="C39" s="44"/>
+      <c r="D39" s="44"/>
+      <c r="E39" s="44"/>
+      <c r="F39" s="45"/>
     </row>
     <row r="40" spans="1:6" customHeight="1" ht="15.75">
-      <c r="A40" s="55"/>
-      <c r="B40" s="51"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="51"/>
-      <c r="E40" s="51"/>
-      <c r="F40" s="52"/>
+      <c r="A40" s="49"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="46"/>
     </row>
     <row r="41" spans="1:6" customHeight="1" ht="16.5">
       <c r="A41" s="3"/>
-      <c r="B41" s="59" t="s">
-        <v>23</v>
-      </c>
-      <c r="C41" s="59"/>
-      <c r="D41" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="E41" s="45"/>
-      <c r="F41" s="46"/>
+      <c r="B41" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" s="34"/>
+      <c r="D41" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="E41" s="40"/>
+      <c r="F41" s="41"/>
     </row>
     <row r="42" spans="1:6" customHeight="1" ht="15.75">
       <c r="A42" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B42" s="60"/>
-      <c r="C42" s="60"/>
-      <c r="D42" s="41"/>
-      <c r="E42" s="41"/>
-      <c r="F42" s="42"/>
+        <v>27</v>
+      </c>
+      <c r="B42" s="35"/>
+      <c r="C42" s="35"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="37"/>
     </row>
     <row r="43" spans="1:6" customHeight="1" ht="15.75">
       <c r="A43" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B43" s="58" t="s">
-        <v>27</v>
-      </c>
-      <c r="C43" s="58"/>
-      <c r="D43" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="E43" s="43"/>
-      <c r="F43" s="44"/>
+      <c r="B43" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C43" s="32"/>
+      <c r="D43" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="E43" s="38"/>
+      <c r="F43" s="39"/>
     </row>
     <row r="44" spans="1:6" customHeight="1" ht="20.25">
       <c r="A44" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B44" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="C44" s="51"/>
-      <c r="D44" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="E44" s="56"/>
-      <c r="F44" s="57"/>
+      <c r="B44" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C44" s="33"/>
+      <c r="D44" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="E44" s="50"/>
+      <c r="F44" s="51"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="true" formatColumns="true" formatRows="true" insertColumns="true" insertRows="true" insertHyperlinks="true" deleteColumns="true" deleteRows="true" selectLockedCells="false" sort="true" autoFilter="true" pivotTables="true" selectUnlockedCells="false"/>
   <mergeCells>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="D42:F42"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="B37:F40"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="E7:F7"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="A9:A10"/>
@@ -1361,6 +1372,18 @@
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A5:F5"/>
+    <mergeCell ref="D42:F42"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="B37:F40"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true" horizontalCentered="true"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
commits March 25, 2020
</commit_message>
<xml_diff>
--- a/export_pr.xlsx
+++ b/export_pr.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
   <si>
     <t>Appendix 60</t>
   </si>
@@ -35,16 +35,16 @@
     <t>Office/Section :</t>
   </si>
   <si>
-    <t>LGCDD-MBRTG</t>
-  </si>
-  <si>
-    <t>PR No.:  2020-03-0164</t>
+    <t>FAD</t>
+  </si>
+  <si>
+    <t>PR No.:  2020-03-0124</t>
   </si>
   <si>
     <t xml:space="preserve">Date: </t>
   </si>
   <si>
-    <t>March 17, 2020</t>
+    <t>March 25, 2020</t>
   </si>
   <si>
     <t xml:space="preserve">Responsibility Center Code : </t>
@@ -68,21 +68,14 @@
     <t>Total Cost</t>
   </si>
   <si>
-    <t>S860</t>
-  </si>
-  <si>
-    <t>piece</t>
-  </si>
-  <si>
-    <t>IEC Material 18x24
-Sintra Board 18x24</t>
-  </si>
-  <si>
-    <t>S859</t>
-  </si>
-  <si>
-    <t>IEC Material 24x36
-Tarpauline</t>
+    <t>S280</t>
+  </si>
+  <si>
+    <t>box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Map Pin/Pin Assrtd Colored
+</t>
   </si>
   <si>
     <t>Total</t>
@@ -91,7 +84,7 @@
     <t>Purpose:</t>
   </si>
   <si>
-    <t>Dissemination of IEC Related to Manila Bay Clean-up, Rehabilitation and Preservation Program Weekly Clean-up</t>
+    <t xml:space="preserve">121212 </t>
   </si>
   <si>
     <t>Requested by:</t>
@@ -106,7 +99,7 @@
     <t>Printed Name :</t>
   </si>
   <si>
-    <t>JAY-AR T. BELTRAN</t>
+    <t>DR. CARINA S. CRUZ</t>
   </si>
   <si>
     <t>NOEL R. BARTOLABAC, CESO V</t>
@@ -115,7 +108,7 @@
     <t>Designation :</t>
   </si>
   <si>
-    <t>OIC - LGCDD Chief</t>
+    <t>FAD Chief</t>
   </si>
   <si>
     <t>Assistant Regional Director</t>
@@ -1046,33 +1039,33 @@
         <v>19</v>
       </c>
       <c r="D11" s="18">
-        <v>67</v>
+        <v>1</v>
       </c>
       <c r="E11" s="26">
-        <v>400</v>
+        <v>65</v>
       </c>
       <c r="F11" s="26">
-        <v>26800</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="2" customFormat="1">
       <c r="A12" s="19" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B12" s="20" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="29" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D12" s="20">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E12" s="27">
-        <v>516</v>
+        <v>65</v>
       </c>
       <c r="F12" s="27">
-        <v>3096</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:6" customHeight="1" ht="30" s="2" customFormat="1">
@@ -1265,19 +1258,19 @@
       <c r="C36" s="22"/>
       <c r="D36" s="22"/>
       <c r="E36" s="24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F36" s="25">
         <f>SUM(F11:F35)</f>
-        <v>29896</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:6" customHeight="1" ht="15.75">
       <c r="A37" s="54" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B37" s="48" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C37" s="48"/>
       <c r="D37" s="48"/>
@@ -1311,18 +1304,18 @@
     <row r="41" spans="1:6" customHeight="1" ht="16.5">
       <c r="A41" s="3"/>
       <c r="B41" s="60" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C41" s="60"/>
       <c r="D41" s="46" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E41" s="46"/>
       <c r="F41" s="47"/>
     </row>
     <row r="42" spans="1:6" customHeight="1" ht="15.75">
       <c r="A42" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B42" s="61"/>
       <c r="C42" s="61"/>
@@ -1332,28 +1325,28 @@
     </row>
     <row r="43" spans="1:6" customHeight="1" ht="15.75">
       <c r="A43" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B43" s="59" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C43" s="59"/>
       <c r="D43" s="44" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E43" s="44"/>
       <c r="F43" s="45"/>
     </row>
     <row r="44" spans="1:6" customHeight="1" ht="20.25">
       <c r="A44" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B44" s="52" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C44" s="52"/>
       <c r="D44" s="57" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E44" s="57"/>
       <c r="F44" s="58"/>

</xml_diff>